<commit_message>
added modification according to must skills total more than 10 and less than 2
</commit_message>
<xml_diff>
--- a/upload_files/Nihad_Azimli_Resume__ticketswap_data_engineer.xlsx
+++ b/upload_files/Nihad_Azimli_Resume__ticketswap_data_engineer.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="84">
   <si>
     <t>CV ID</t>
   </si>
@@ -55,7 +55,7 @@
     <t>ticketswap_data_engineer.txt</t>
   </si>
   <si>
-    <t>82.63</t>
+    <t>98.80</t>
   </si>
   <si>
     <t>data engineer : 2</t>
@@ -229,43 +229,40 @@
     <t>ansible : 1</t>
   </si>
   <si>
+    <t>docker : 3</t>
+  </si>
+  <si>
+    <t>bi : 1</t>
+  </si>
+  <si>
+    <t>aws : 4</t>
+  </si>
+  <si>
+    <t>kubernetes : 2</t>
+  </si>
+  <si>
+    <t>etl : 4</t>
+  </si>
+  <si>
     <t>mongodb : 1</t>
   </si>
   <si>
-    <t>python : 2</t>
+    <t>100.0</t>
+  </si>
+  <si>
+    <t>go : 1</t>
+  </si>
+  <si>
+    <t>redshift : 2</t>
   </si>
   <si>
     <t>kinesis : 1</t>
   </si>
   <si>
-    <t>aws : 4</t>
-  </si>
-  <si>
-    <t>go : 1</t>
-  </si>
-  <si>
     <t>spark : 1</t>
   </si>
   <si>
-    <t>design : 4</t>
-  </si>
-  <si>
-    <t>kubernetes : 2</t>
-  </si>
-  <si>
-    <t>bi : 1</t>
-  </si>
-  <si>
-    <t>docker : 3</t>
-  </si>
-  <si>
-    <t>redshift : 2</t>
-  </si>
-  <si>
-    <t>etl : 4</t>
-  </si>
-  <si>
-    <t>78.12</t>
+    <t>50.0</t>
   </si>
   <si>
     <t>0.0</t>
@@ -680,13 +677,16 @@
         <v>71</v>
       </c>
       <c r="G2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K2" t="s">
         <v>83</v>
-      </c>
-      <c r="I2" t="s">
-        <v>84</v>
-      </c>
-      <c r="K2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -694,7 +694,10 @@
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>45</v>
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -704,13 +707,19 @@
       <c r="F4" t="s">
         <v>72</v>
       </c>
+      <c r="H4" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="5" spans="1:11">
       <c r="E5" t="s">
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>73</v>
+      </c>
+      <c r="H5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -718,7 +727,10 @@
         <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>73</v>
+        <v>45</v>
+      </c>
+      <c r="H6" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -726,7 +738,10 @@
         <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>51</v>
+        <v>74</v>
+      </c>
+      <c r="H7" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -734,7 +749,7 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -742,7 +757,7 @@
         <v>21</v>
       </c>
       <c r="F9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -750,7 +765,7 @@
         <v>22</v>
       </c>
       <c r="F10" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -758,134 +773,110 @@
         <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="E12" t="s">
         <v>24</v>
       </c>
-      <c r="F12" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="13" spans="1:11">
       <c r="E13" t="s">
         <v>25</v>
       </c>
-      <c r="F13" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="14" spans="1:11">
       <c r="E14" t="s">
         <v>26</v>
       </c>
-      <c r="F14" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="15" spans="1:11">
       <c r="E15" t="s">
         <v>27</v>
       </c>
-      <c r="F15" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="16" spans="1:11">
       <c r="E16" t="s">
         <v>28</v>
       </c>
-      <c r="F16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="5:6">
+    </row>
+    <row r="17" spans="5:5">
       <c r="E17" t="s">
         <v>29</v>
       </c>
-      <c r="F17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="5:6">
+    </row>
+    <row r="18" spans="5:5">
       <c r="E18" t="s">
         <v>30</v>
       </c>
-      <c r="F18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="5:6">
+    </row>
+    <row r="19" spans="5:5">
       <c r="E19" t="s">
         <v>31</v>
       </c>
-      <c r="F19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="5:6">
+    </row>
+    <row r="20" spans="5:5">
       <c r="E20" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="5:6">
+    <row r="21" spans="5:5">
       <c r="E21" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="5:6">
+    <row r="22" spans="5:5">
       <c r="E22" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="5:6">
+    <row r="23" spans="5:5">
       <c r="E23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="5:6">
+    <row r="24" spans="5:5">
       <c r="E24" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="5:6">
+    <row r="25" spans="5:5">
       <c r="E25" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="5:6">
+    <row r="26" spans="5:5">
       <c r="E26" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="5:6">
+    <row r="27" spans="5:5">
       <c r="E27" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="5:6">
+    <row r="28" spans="5:5">
       <c r="E28" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="5:6">
+    <row r="29" spans="5:5">
       <c r="E29" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="5:6">
+    <row r="30" spans="5:5">
       <c r="E30" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="5:6">
+    <row r="31" spans="5:5">
       <c r="E31" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="5:6">
+    <row r="32" spans="5:5">
       <c r="E32" t="s">
         <v>44</v>
       </c>

</xml_diff>